<commit_message>
Update de 3 jours (+ poo zone budget)
</commit_message>
<xml_diff>
--- a/codes_tests/data/piezos/pz_hydriad.xlsx
+++ b/codes_tests/data/piezos/pz_hydriad.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmal\Documents\GitHub\TM_Ludovic_Schorpp\codes_tests\data\piezos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0998ECE8-B85A-4DDD-B8F4-5B8605EB2448}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F52F9C6-3F8D-4398-9226-5CE1BBB58C60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1635,7 +1635,7 @@
   <dimension ref="A1:E193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>